<commit_message>
Versión final y con corrección de estilo de CN_08_04_CO
Se incluyen las correcciones al esqueleto de guión y a la guía
didáctica.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion04/EsqueletoGuion_CN_08_04_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion04/EsqueletoGuion_CN_08_04_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="1455" windowWidth="19440" windowHeight="11700" tabRatio="729" activeTab="4"/>
+    <workbookView xWindow="3405" yWindow="1455" windowWidth="19440" windowHeight="11700" tabRatio="729" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -1578,7 +1578,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1661,8 +1661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:D14"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1964,7 +1964,7 @@
         <v>54</v>
       </c>
       <c r="F14">
-        <v>200</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2409,7 +2409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="615" topLeftCell="A73" activePane="bottomLeft"/>
       <selection pane="bottomLeft" activeCell="A84" sqref="A84"/>
     </sheetView>
@@ -2742,7 +2742,7 @@
       </c>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -2762,7 +2762,7 @@
       </c>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -2842,7 +2842,7 @@
       </c>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -2862,7 +2862,7 @@
       </c>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -3002,7 +3002,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>19</v>
       </c>
@@ -3019,7 +3019,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>19</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Documentos CN_08_04_CO con revisión de estilo
Última versión de los documentos, con las correcciones de estilo
completas
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion04/EsqueletoGuion_CN_08_04_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion04/EsqueletoGuion_CN_08_04_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="1455" windowWidth="19440" windowHeight="11700" tabRatio="729" activeTab="1"/>
+    <workbookView xWindow="3405" yWindow="1455" windowWidth="19440" windowHeight="11700" tabRatio="729" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -1578,7 +1578,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1661,7 +1661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -2409,9 +2409,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="615" topLeftCell="A73" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="A84" sqref="A84"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="615" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Corrección en texto y esqueleto de guión
Faltaba el texto antes de la subsecciones consolidación y de la sección
competencias. Se agregaron y se hizo el cambio en el esqueleto de guión
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion04/EsqueletoGuion_CN_08_04_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion04/EsqueletoGuion_CN_08_04_CO.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="111">
   <si>
     <t>FICHA</t>
   </si>
@@ -1578,7 +1578,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2407,11 +2407,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I83"/>
+  <dimension ref="A1:I90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="615" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2547,7 +2547,7 @@
       <c r="G6" s="9"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -2559,32 +2559,34 @@
         <v>67</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
-      <c r="H7" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
+        <v>62</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>68</v>
+      </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
-      <c r="H8" s="5"/>
+      <c r="H8" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -2593,13 +2595,11 @@
       <c r="B9" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>63</v>
-      </c>
+      <c r="C9" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="5"/>
@@ -2616,7 +2616,7 @@
         <v>43</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
@@ -2633,13 +2633,11 @@
       <c r="D11" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>63</v>
-      </c>
+      <c r="E11" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2658,7 +2656,7 @@
         <v>70</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H12" s="5"/>
     </row>
@@ -2675,10 +2673,10 @@
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H13" s="5"/>
     </row>
@@ -2698,7 +2696,7 @@
         <v>71</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H14" s="5"/>
     </row>
@@ -2715,10 +2713,10 @@
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H15" s="5"/>
     </row>
@@ -2738,7 +2736,7 @@
         <v>72</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H16" s="5"/>
     </row>
@@ -2755,10 +2753,10 @@
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H17" s="5"/>
     </row>
@@ -2778,7 +2776,7 @@
         <v>73</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H18" s="5"/>
     </row>
@@ -2795,10 +2793,10 @@
       </c>
       <c r="E19" s="9"/>
       <c r="F19" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H19" s="5"/>
     </row>
@@ -2818,7 +2816,7 @@
         <v>74</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H20" s="5"/>
     </row>
@@ -2838,11 +2836,11 @@
         <v>74</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -2855,10 +2853,10 @@
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="9" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="H22" s="5"/>
     </row>
@@ -2878,16 +2876,11 @@
         <v>81</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -2896,14 +2889,21 @@
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="5"/>
+        <v>43</v>
+      </c>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -2917,7 +2917,7 @@
         <v>76</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
@@ -2930,12 +2930,16 @@
       <c r="B26" s="8" t="s">
         <v>29</v>
       </c>
+      <c r="C26" s="8"/>
       <c r="D26" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="E26" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -2948,7 +2952,7 @@
         <v>76</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -2961,11 +2965,8 @@
       <c r="D28" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="F28" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>63</v>
+      <c r="E28" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -2982,7 +2983,7 @@
         <v>77</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -2999,7 +3000,7 @@
         <v>77</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -3013,7 +3014,7 @@
         <v>76</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>63</v>
@@ -3033,7 +3034,7 @@
         <v>78</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -3047,13 +3048,13 @@
         <v>76</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>19</v>
       </c>
@@ -3064,7 +3065,7 @@
         <v>76</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>63</v>
@@ -3081,7 +3082,7 @@
         <v>76</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>63</v>
@@ -3101,27 +3102,24 @@
         <v>75</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>19</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H37" t="s">
-        <v>82</v>
-      </c>
-      <c r="I37" s="9" t="s">
-        <v>25</v>
+      <c r="D37" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -3131,17 +3129,11 @@
       <c r="B38" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="9" t="s">
         <v>67</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H38" t="s">
-        <v>83</v>
-      </c>
-      <c r="I38" s="5" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -3149,10 +3141,19 @@
         <v>19</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>63</v>
+        <v>29</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H39" t="s">
+        <v>82</v>
+      </c>
+      <c r="I39" s="9" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -3160,13 +3161,19 @@
         <v>19</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>63</v>
+        <v>68</v>
+      </c>
+      <c r="H40" t="s">
+        <v>83</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -3176,11 +3183,8 @@
       <c r="B41" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>85</v>
+      <c r="C41" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -3191,7 +3195,7 @@
         <v>35</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>63</v>
@@ -3205,10 +3209,10 @@
         <v>35</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -3219,55 +3223,58 @@
         <v>35</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H44" t="s">
-        <v>87</v>
-      </c>
-      <c r="I44" s="9" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>19</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>63</v>
+      <c r="B45" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>19</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>66</v>
+      <c r="B46" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>19</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>64</v>
+      <c r="B47" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="H47" t="s">
-        <v>36</v>
-      </c>
-      <c r="I47" s="5" t="s">
-        <v>25</v>
+        <v>87</v>
+      </c>
+      <c r="I47" s="9" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -3277,17 +3284,8 @@
       <c r="B48" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D48" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H48" t="s">
-        <v>88</v>
-      </c>
-      <c r="I48" s="5" t="s">
-        <v>27</v>
+      <c r="C48" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -3295,30 +3293,27 @@
         <v>19</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>19</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>63</v>
+        <v>38</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H50" t="s">
+        <v>36</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -3326,10 +3321,10 @@
         <v>19</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>63</v>
@@ -3340,13 +3335,19 @@
         <v>19</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>63</v>
+        <v>38</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H52" t="s">
+        <v>88</v>
+      </c>
+      <c r="I52" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -3356,14 +3357,11 @@
       <c r="B53" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D53" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C53" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>19</v>
       </c>
@@ -3371,9 +3369,15 @@
         <v>44</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E54" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G54" s="3" t="s">
         <v>63</v>
       </c>
     </row>
@@ -3385,7 +3389,7 @@
         <v>44</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>63</v>
@@ -3399,10 +3403,10 @@
         <v>44</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -3413,16 +3417,10 @@
         <v>44</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H57" t="s">
-        <v>39</v>
-      </c>
-      <c r="I57" s="5" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -3433,7 +3431,7 @@
         <v>44</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>63</v>
@@ -3449,10 +3447,7 @@
       <c r="D59" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="F59" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="G59" s="3" t="s">
+      <c r="E59" s="3" t="s">
         <v>63</v>
       </c>
     </row>
@@ -3466,11 +3461,8 @@
       <c r="D60" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="F60" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G60" s="3" t="s">
-        <v>63</v>
+      <c r="E60" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -3483,11 +3475,14 @@
       <c r="D61" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="F61" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="G61" s="3" t="s">
-        <v>63</v>
+      <c r="E61" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H61" t="s">
+        <v>39</v>
+      </c>
+      <c r="I61" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -3500,10 +3495,7 @@
       <c r="D62" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="F62" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="G62" s="3" t="s">
+      <c r="E62" s="3" t="s">
         <v>63</v>
       </c>
     </row>
@@ -3518,7 +3510,7 @@
         <v>92</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G63" s="3" t="s">
         <v>63</v>
@@ -3535,16 +3527,10 @@
         <v>92</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H64" t="s">
-        <v>97</v>
-      </c>
-      <c r="I64" s="5" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -3558,16 +3544,10 @@
         <v>92</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H65" t="s">
-        <v>98</v>
-      </c>
-      <c r="I65" s="5" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -3578,9 +3558,12 @@
         <v>44</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E66" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G66" s="3" t="s">
         <v>63</v>
       </c>
     </row>
@@ -3592,16 +3575,13 @@
         <v>44</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H67" t="s">
-        <v>110</v>
-      </c>
-      <c r="I67" s="5" t="s">
-        <v>25</v>
+        <v>92</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -3612,15 +3592,18 @@
         <v>44</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>68</v>
+        <v>92</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="H68" t="s">
-        <v>100</v>
-      </c>
-      <c r="I68" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="I68" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3629,10 +3612,22 @@
         <v>19</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>63</v>
+        <v>44</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H69" t="s">
+        <v>98</v>
+      </c>
+      <c r="I69" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -3640,10 +3635,10 @@
         <v>19</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>63</v>
@@ -3654,13 +3649,19 @@
         <v>19</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>63</v>
+        <v>68</v>
+      </c>
+      <c r="H71" t="s">
+        <v>110</v>
+      </c>
+      <c r="I71" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -3668,13 +3669,10 @@
         <v>19</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -3682,13 +3680,19 @@
         <v>19</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>102</v>
+        <v>67</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>63</v>
+        <v>68</v>
+      </c>
+      <c r="H73" t="s">
+        <v>100</v>
+      </c>
+      <c r="I73" s="9" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -3698,17 +3702,8 @@
       <c r="B74" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D74" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H74" t="s">
-        <v>46</v>
-      </c>
-      <c r="I74" s="5" t="s">
-        <v>25</v>
+      <c r="C74" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -3719,7 +3714,7 @@
         <v>46</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>63</v>
@@ -3733,16 +3728,10 @@
         <v>46</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H76" t="s">
-        <v>103</v>
-      </c>
-      <c r="I76" s="5" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -3753,16 +3742,10 @@
         <v>46</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>67</v>
+        <v>102</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H77" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="I77" s="9" t="s">
-        <v>25</v>
+        <v>85</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -3773,16 +3756,10 @@
         <v>46</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>67</v>
+        <v>102</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H78" t="s">
-        <v>59</v>
-      </c>
-      <c r="I78" s="5" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -3793,13 +3770,13 @@
         <v>46</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>67</v>
+        <v>102</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H79" t="s">
-        <v>105</v>
+        <v>46</v>
       </c>
       <c r="I79" s="5" t="s">
         <v>25</v>
@@ -3810,16 +3787,13 @@
         <v>19</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H80" t="s">
-        <v>107</v>
-      </c>
-      <c r="I80" s="5" t="s">
-        <v>25</v>
+        <v>46</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -3827,13 +3801,16 @@
         <v>19</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>68</v>
+        <v>46</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="H81" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="I81" s="5" t="s">
         <v>25</v>
@@ -3844,13 +3821,13 @@
         <v>19</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I82" s="5" t="s">
-        <v>27</v>
+        <v>46</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
@@ -3858,12 +3835,131 @@
         <v>19</v>
       </c>
       <c r="B83" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H83" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I83" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>19</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H84" t="s">
+        <v>59</v>
+      </c>
+      <c r="I84" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>19</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H85" t="s">
+        <v>105</v>
+      </c>
+      <c r="I85" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>19</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>19</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H87" t="s">
+        <v>107</v>
+      </c>
+      <c r="I87" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>19</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H88" t="s">
+        <v>108</v>
+      </c>
+      <c r="I88" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>19</v>
+      </c>
+      <c r="B89" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="C89" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I89" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>19</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C90" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I83" s="5" t="s">
+      <c r="I90" s="5" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Corrección en nombres de recursos
Corregidos los nombres en el esqueleto del guión
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion04/EsqueletoGuion_CN_08_04_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion04/EsqueletoGuion_CN_08_04_CO.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="3405" yWindow="1455" windowWidth="19440" windowHeight="11700" tabRatio="729" activeTab="4"/>
@@ -13,7 +13,7 @@
     <sheet name="CUADERNO DEL PROFESOR" sheetId="15" r:id="rId4"/>
     <sheet name="CUADERNO DE ESTUDIO" sheetId="16" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="102">
   <si>
     <t>FICHA</t>
   </si>
@@ -136,9 +136,6 @@
     <t>La reproducción en microorganismos</t>
   </si>
   <si>
-    <t>Reproducción del hongo Philobolus</t>
-  </si>
-  <si>
     <t>Los reinos de móneras, protoctistas y hongos</t>
   </si>
   <si>
@@ -274,9 +271,6 @@
     <t>Ventajas y desventajas de la reproducción asexual</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: Los tipos de reproducción en los seres vivos</t>
-  </si>
-  <si>
     <t>Refuerza tu aprendizaje: Ventajas y desventajas de los tipos de reproducción</t>
   </si>
   <si>
@@ -292,9 +286,6 @@
     <t>Refuerza tu aprendizaje: La reproducción en microorganismos</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: La reproducción en hongos</t>
-  </si>
-  <si>
     <t>La alternancia de generaciones</t>
   </si>
   <si>
@@ -319,18 +310,9 @@
     <t>La germinación</t>
   </si>
   <si>
-    <t>Alternancia de generaciones en una angiosperma</t>
-  </si>
-  <si>
-    <t>La reproducción sexual en las plantas</t>
-  </si>
-  <si>
     <t>Otras formas de reproducción asexual en plantas</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: La reproducción en plantas</t>
-  </si>
-  <si>
     <t>La reproducción asexual en animales</t>
   </si>
   <si>
@@ -340,25 +322,16 @@
     <t>La reproducción alternante en animales</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: Los tipos de reproducción en animales</t>
-  </si>
-  <si>
-    <t>La función de la reproducción</t>
-  </si>
-  <si>
     <t>Competencias</t>
   </si>
   <si>
-    <t>Competencias: Relaciona los tipos de reproducción con organismos en los que se lleva a cabo</t>
-  </si>
-  <si>
-    <t>Competencias: Analiza el crecimiento bacteriano</t>
-  </si>
-  <si>
     <t>Fin de unidad</t>
   </si>
   <si>
-    <t>Relaciona los tipos de reproducción asexual en las plantas con su definición</t>
+    <t>Refuerza tu aprendizaje: La reproducción de los hongos</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: La reproducción de las plantas</t>
   </si>
 </sst>
 </file>
@@ -1578,7 +1551,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1662,7 +1635,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1711,7 +1684,7 @@
         <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F2">
         <v>4</v>
@@ -1731,13 +1704,13 @@
         <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" t="s">
         <v>53</v>
-      </c>
-      <c r="E3" t="s">
-        <v>54</v>
       </c>
       <c r="F3">
         <v>7</v>
@@ -1745,19 +1718,19 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
         <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F4">
         <v>9</v>
@@ -1765,19 +1738,19 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
         <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F5">
         <v>10</v>
@@ -1785,19 +1758,19 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
         <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F6">
         <v>11</v>
@@ -1805,19 +1778,19 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
         <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F7">
         <v>12</v>
@@ -1825,19 +1798,19 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
         <v>31</v>
       </c>
       <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
         <v>45</v>
       </c>
-      <c r="D8" t="s">
-        <v>46</v>
-      </c>
       <c r="E8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F8">
         <v>14</v>
@@ -1854,10 +1827,10 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F9">
         <v>15</v>
@@ -1866,19 +1839,19 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
         <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F10">
         <v>16</v>
@@ -1887,19 +1860,19 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
         <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F11">
         <v>17</v>
@@ -1908,19 +1881,19 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
         <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F12">
         <v>18</v>
@@ -1938,10 +1911,10 @@
         <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F13">
         <v>19</v>
@@ -1955,13 +1928,13 @@
         <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F14">
         <v>20</v>
@@ -1983,7 +1956,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:A10"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2038,7 +2011,7 @@
     </row>
     <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
         <v>27</v>
@@ -2049,7 +2022,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="B6" t="s">
         <v>27</v>
@@ -2060,7 +2033,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>100</v>
       </c>
       <c r="B7" t="s">
         <v>27</v>
@@ -2071,7 +2044,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>101</v>
       </c>
       <c r="B8" t="s">
         <v>27</v>
@@ -2082,7 +2055,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
         <v>27</v>
@@ -2093,7 +2066,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
         <v>27</v>
@@ -2124,7 +2097,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2216,7 +2189,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>25</v>
@@ -2227,7 +2200,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>27</v>
@@ -2238,7 +2211,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>25</v>
@@ -2249,7 +2222,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>25</v>
@@ -2260,7 +2233,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>25</v>
@@ -2271,7 +2244,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>25</v>
@@ -2282,7 +2255,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>27</v>
@@ -2293,7 +2266,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>25</v>
@@ -2304,7 +2277,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>25</v>
@@ -2315,7 +2288,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>25</v>
@@ -2326,7 +2299,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>25</v>
@@ -2337,7 +2310,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>25</v>
@@ -2348,7 +2321,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>25</v>
@@ -2359,7 +2332,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>25</v>
@@ -2370,7 +2343,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>27</v>
@@ -2381,7 +2354,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>27</v>
@@ -2409,9 +2382,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="615" activePane="bottomLeft"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="615" topLeftCell="A73" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="H88" sqref="H88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2461,10 +2434,10 @@
         <v>19</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -2477,10 +2450,10 @@
         <v>19</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -2498,14 +2471,14 @@
         <v>19</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
@@ -2516,14 +2489,14 @@
         <v>19</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>65</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>66</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
@@ -2534,14 +2507,14 @@
         <v>19</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
@@ -2552,14 +2525,14 @@
         <v>19</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
@@ -2570,14 +2543,14 @@
         <v>19</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>67</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>68</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
@@ -2596,7 +2569,7 @@
         <v>29</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
@@ -2613,10 +2586,10 @@
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
@@ -2631,10 +2604,10 @@
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
@@ -2649,14 +2622,14 @@
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H12" s="5"/>
     </row>
@@ -2669,14 +2642,14 @@
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H13" s="5"/>
     </row>
@@ -2689,14 +2662,14 @@
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H14" s="5"/>
     </row>
@@ -2709,14 +2682,14 @@
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H15" s="5"/>
     </row>
@@ -2729,14 +2702,14 @@
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E16" s="9"/>
       <c r="F16" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H16" s="5"/>
     </row>
@@ -2749,14 +2722,14 @@
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H17" s="5"/>
     </row>
@@ -2769,14 +2742,14 @@
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H18" s="5"/>
     </row>
@@ -2789,14 +2762,14 @@
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E19" s="9"/>
       <c r="F19" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H19" s="5"/>
     </row>
@@ -2809,14 +2782,14 @@
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H20" s="5"/>
     </row>
@@ -2829,14 +2802,14 @@
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H21" s="5"/>
     </row>
@@ -2849,14 +2822,14 @@
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H22" s="5"/>
     </row>
@@ -2869,14 +2842,14 @@
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E23" s="9"/>
       <c r="F23" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H23" s="5"/>
     </row>
@@ -2889,14 +2862,14 @@
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E24" s="9"/>
       <c r="F24" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H24" s="5" t="s">
         <v>28</v>
@@ -2914,10 +2887,10 @@
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
@@ -2932,10 +2905,10 @@
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
@@ -2949,10 +2922,10 @@
         <v>29</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -2963,10 +2936,10 @@
         <v>29</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -2977,13 +2950,13 @@
         <v>29</v>
       </c>
       <c r="D29" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F29" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="G29" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -2994,13 +2967,13 @@
         <v>29</v>
       </c>
       <c r="D30" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F30" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F30" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="G30" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -3011,13 +2984,13 @@
         <v>29</v>
       </c>
       <c r="D31" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F31" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F31" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="G31" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -3028,13 +3001,13 @@
         <v>29</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -3045,13 +3018,13 @@
         <v>29</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -3062,13 +3035,13 @@
         <v>29</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3079,13 +3052,13 @@
         <v>29</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3096,13 +3069,13 @@
         <v>29</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3113,13 +3086,13 @@
         <v>29</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -3130,10 +3103,10 @@
         <v>29</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -3144,13 +3117,13 @@
         <v>29</v>
       </c>
       <c r="D39" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E39" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E39" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="H39" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="I39" s="9" t="s">
         <v>25</v>
@@ -3164,13 +3137,13 @@
         <v>29</v>
       </c>
       <c r="D40" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E40" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E40" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="H40" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I40" s="5" t="s">
         <v>27</v>
@@ -3184,7 +3157,7 @@
         <v>35</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -3195,10 +3168,10 @@
         <v>35</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -3209,10 +3182,10 @@
         <v>35</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -3223,10 +3196,10 @@
         <v>35</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -3237,10 +3210,10 @@
         <v>35</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -3251,10 +3224,10 @@
         <v>35</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -3265,13 +3238,13 @@
         <v>35</v>
       </c>
       <c r="D47" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E47" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E47" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="H47" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I47" s="9" t="s">
         <v>27</v>
@@ -3282,10 +3255,10 @@
         <v>19</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -3293,10 +3266,10 @@
         <v>19</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -3304,13 +3277,13 @@
         <v>19</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H50" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="I50" s="5" t="s">
         <v>25</v>
@@ -3321,13 +3294,13 @@
         <v>19</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -3335,16 +3308,16 @@
         <v>19</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D52" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E52" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E52" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="H52" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="I52" s="5" t="s">
         <v>27</v>
@@ -3355,10 +3328,10 @@
         <v>19</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3366,19 +3339,19 @@
         <v>19</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -3386,13 +3359,13 @@
         <v>19</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -3400,13 +3373,13 @@
         <v>19</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -3414,13 +3387,13 @@
         <v>19</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -3428,13 +3401,13 @@
         <v>19</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -3442,13 +3415,13 @@
         <v>19</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -3456,13 +3429,13 @@
         <v>19</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -3470,16 +3443,16 @@
         <v>19</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H61" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I61" s="5" t="s">
         <v>25</v>
@@ -3490,13 +3463,13 @@
         <v>19</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -3504,16 +3477,16 @@
         <v>19</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -3521,16 +3494,16 @@
         <v>19</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -3538,16 +3511,16 @@
         <v>19</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -3555,16 +3528,16 @@
         <v>19</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D66" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F66" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="F66" s="3" t="s">
-        <v>95</v>
-      </c>
       <c r="G66" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -3572,16 +3545,16 @@
         <v>19</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -3589,19 +3562,19 @@
         <v>19</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H68" t="s">
-        <v>97</v>
+        <v>41</v>
       </c>
       <c r="I68" s="5" t="s">
         <v>25</v>
@@ -3612,19 +3585,19 @@
         <v>19</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H69" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="I69" s="5" t="s">
         <v>25</v>
@@ -3635,13 +3608,13 @@
         <v>19</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -3649,16 +3622,16 @@
         <v>19</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H71" t="s">
-        <v>110</v>
+        <v>56</v>
       </c>
       <c r="I71" s="5" t="s">
         <v>25</v>
@@ -3669,10 +3642,10 @@
         <v>19</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -3680,16 +3653,16 @@
         <v>19</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D73" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E73" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E73" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="H73" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I73" s="9" t="s">
         <v>25</v>
@@ -3700,10 +3673,10 @@
         <v>19</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -3711,13 +3684,13 @@
         <v>19</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -3725,13 +3698,13 @@
         <v>19</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -3739,13 +3712,13 @@
         <v>19</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -3753,13 +3726,13 @@
         <v>19</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -3767,16 +3740,16 @@
         <v>19</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H79" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I79" s="5" t="s">
         <v>25</v>
@@ -3787,13 +3760,13 @@
         <v>19</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -3801,16 +3774,16 @@
         <v>19</v>
       </c>
       <c r="B81" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H81" t="s">
         <v>46</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E81" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H81" t="s">
-        <v>103</v>
       </c>
       <c r="I81" s="5" t="s">
         <v>25</v>
@@ -3821,13 +3794,13 @@
         <v>19</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
@@ -3835,16 +3808,16 @@
         <v>19</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D83" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E83" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E83" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="H83" s="3" t="s">
-        <v>104</v>
+        <v>47</v>
       </c>
       <c r="I83" s="9" t="s">
         <v>25</v>
@@ -3855,16 +3828,16 @@
         <v>19</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D84" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E84" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E84" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="H84" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I84" s="5" t="s">
         <v>25</v>
@@ -3875,16 +3848,16 @@
         <v>19</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D85" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E85" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E85" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="H85" t="s">
-        <v>105</v>
+        <v>59</v>
       </c>
       <c r="I85" s="5" t="s">
         <v>25</v>
@@ -3895,10 +3868,10 @@
         <v>19</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
@@ -3906,13 +3879,13 @@
         <v>19</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H87" t="s">
-        <v>107</v>
+        <v>48</v>
       </c>
       <c r="I87" s="5" t="s">
         <v>25</v>
@@ -3923,13 +3896,13 @@
         <v>19</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H88" t="s">
-        <v>108</v>
+        <v>60</v>
       </c>
       <c r="I88" s="5" t="s">
         <v>25</v>
@@ -3940,10 +3913,10 @@
         <v>19</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I89" s="5" t="s">
         <v>27</v>
@@ -3954,10 +3927,10 @@
         <v>19</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I90" s="5" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Segunda corrección nombres esqueleto de guión
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion04/EsqueletoGuion_CN_08_04_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion04/EsqueletoGuion_CN_08_04_CO.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="101">
   <si>
     <t>FICHA</t>
   </si>
@@ -128,9 +128,6 @@
   </si>
   <si>
     <t>Selecciona cómo se reproducen estos organismos</t>
-  </si>
-  <si>
-    <t>Ventajas y desventajas de los tipos de reproducción</t>
   </si>
   <si>
     <t>La reproducción en microorganismos</t>
@@ -1551,7 +1548,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1635,7 +1632,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1684,7 +1681,7 @@
         <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F2">
         <v>4</v>
@@ -1704,13 +1701,13 @@
         <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" t="s">
         <v>52</v>
-      </c>
-      <c r="E3" t="s">
-        <v>53</v>
       </c>
       <c r="F3">
         <v>7</v>
@@ -1718,19 +1715,19 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
         <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F4">
         <v>9</v>
@@ -1738,19 +1735,19 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
         <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F5">
         <v>10</v>
@@ -1758,19 +1755,19 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
         <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F6">
         <v>11</v>
@@ -1778,19 +1775,19 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
         <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F7">
         <v>12</v>
@@ -1798,19 +1795,19 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
         <v>31</v>
       </c>
       <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
         <v>44</v>
       </c>
-      <c r="D8" t="s">
-        <v>45</v>
-      </c>
       <c r="E8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F8">
         <v>14</v>
@@ -1827,10 +1824,10 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F9">
         <v>15</v>
@@ -1839,19 +1836,19 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
         <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F10">
         <v>16</v>
@@ -1860,19 +1857,19 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
         <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F11">
         <v>17</v>
@@ -1881,19 +1878,19 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
         <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F12">
         <v>18</v>
@@ -1911,10 +1908,10 @@
         <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F13">
         <v>19</v>
@@ -1928,13 +1925,13 @@
         <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F14">
         <v>20</v>
@@ -1956,7 +1953,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2011,7 +2008,7 @@
     </row>
     <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
         <v>27</v>
@@ -2022,7 +2019,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B6" t="s">
         <v>27</v>
@@ -2033,7 +2030,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
         <v>27</v>
@@ -2044,7 +2041,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B8" t="s">
         <v>27</v>
@@ -2055,7 +2052,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
         <v>27</v>
@@ -2066,7 +2063,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
         <v>27</v>
@@ -2097,7 +2094,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2167,7 +2164,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>80</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>27</v>
@@ -2178,7 +2175,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>84</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>27</v>
@@ -2189,7 +2186,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>25</v>
@@ -2200,7 +2197,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>99</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>27</v>
@@ -2211,7 +2208,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>25</v>
@@ -2222,7 +2219,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>25</v>
@@ -2233,7 +2230,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>25</v>
@@ -2244,7 +2241,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>25</v>
@@ -2255,7 +2252,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>100</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>27</v>
@@ -2266,7 +2263,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>25</v>
@@ -2277,7 +2274,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>25</v>
@@ -2288,7 +2285,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>25</v>
@@ -2299,7 +2296,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>25</v>
@@ -2310,7 +2307,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>25</v>
@@ -2321,7 +2318,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>25</v>
@@ -2332,7 +2329,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>25</v>
@@ -2343,7 +2340,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>27</v>
@@ -2354,7 +2351,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>27</v>
@@ -2382,9 +2379,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="615" topLeftCell="A73" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="H88" sqref="H88"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="615" activePane="bottomLeft"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2434,10 +2431,10 @@
         <v>19</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -2450,10 +2447,10 @@
         <v>19</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -2471,14 +2468,14 @@
         <v>19</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
@@ -2489,14 +2486,14 @@
         <v>19</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>64</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>65</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
@@ -2507,14 +2504,14 @@
         <v>19</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
@@ -2525,14 +2522,14 @@
         <v>19</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
@@ -2543,14 +2540,14 @@
         <v>19</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>67</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
@@ -2569,7 +2566,7 @@
         <v>29</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
@@ -2586,10 +2583,10 @@
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
@@ -2604,10 +2601,10 @@
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
@@ -2622,14 +2619,14 @@
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H12" s="5"/>
     </row>
@@ -2642,14 +2639,14 @@
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H13" s="5"/>
     </row>
@@ -2662,14 +2659,14 @@
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H14" s="5"/>
     </row>
@@ -2682,14 +2679,14 @@
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H15" s="5"/>
     </row>
@@ -2702,14 +2699,14 @@
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E16" s="9"/>
       <c r="F16" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H16" s="5"/>
     </row>
@@ -2722,14 +2719,14 @@
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H17" s="5"/>
     </row>
@@ -2742,14 +2739,14 @@
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H18" s="5"/>
     </row>
@@ -2762,14 +2759,14 @@
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E19" s="9"/>
       <c r="F19" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H19" s="5"/>
     </row>
@@ -2782,14 +2779,14 @@
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H20" s="5"/>
     </row>
@@ -2802,14 +2799,14 @@
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H21" s="5"/>
     </row>
@@ -2822,14 +2819,14 @@
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H22" s="5"/>
     </row>
@@ -2842,14 +2839,14 @@
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E23" s="9"/>
       <c r="F23" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H23" s="5"/>
     </row>
@@ -2862,14 +2859,14 @@
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E24" s="9"/>
       <c r="F24" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H24" s="5" t="s">
         <v>28</v>
@@ -2887,10 +2884,10 @@
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
@@ -2905,10 +2902,10 @@
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
@@ -2922,10 +2919,10 @@
         <v>29</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -2936,10 +2933,10 @@
         <v>29</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -2950,13 +2947,13 @@
         <v>29</v>
       </c>
       <c r="D29" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F29" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="G29" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -2967,13 +2964,13 @@
         <v>29</v>
       </c>
       <c r="D30" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F30" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F30" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="G30" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -2984,13 +2981,13 @@
         <v>29</v>
       </c>
       <c r="D31" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F31" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F31" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="G31" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -3001,13 +2998,13 @@
         <v>29</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -3018,13 +3015,13 @@
         <v>29</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -3035,13 +3032,13 @@
         <v>29</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3052,13 +3049,13 @@
         <v>29</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3069,13 +3066,13 @@
         <v>29</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3086,13 +3083,13 @@
         <v>29</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -3103,10 +3100,10 @@
         <v>29</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -3117,10 +3114,10 @@
         <v>29</v>
       </c>
       <c r="D39" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E39" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="H39" t="s">
         <v>33</v>
@@ -3137,13 +3134,13 @@
         <v>29</v>
       </c>
       <c r="D40" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E40" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E40" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="H40" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I40" s="5" t="s">
         <v>27</v>
@@ -3154,10 +3151,10 @@
         <v>19</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -3165,13 +3162,13 @@
         <v>19</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -3179,13 +3176,13 @@
         <v>19</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D43" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E43" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -3193,13 +3190,13 @@
         <v>19</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -3207,13 +3204,13 @@
         <v>19</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -3221,13 +3218,13 @@
         <v>19</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -3235,16 +3232,16 @@
         <v>19</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D47" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E47" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E47" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="H47" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I47" s="9" t="s">
         <v>27</v>
@@ -3255,10 +3252,10 @@
         <v>19</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -3266,10 +3263,10 @@
         <v>19</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -3277,13 +3274,13 @@
         <v>19</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H50" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I50" s="5" t="s">
         <v>25</v>
@@ -3294,13 +3291,13 @@
         <v>19</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -3308,16 +3305,16 @@
         <v>19</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D52" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E52" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E52" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="H52" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I52" s="5" t="s">
         <v>27</v>
@@ -3328,10 +3325,10 @@
         <v>19</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3339,19 +3336,19 @@
         <v>19</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D54" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F54" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E54" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="G54" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -3359,13 +3356,13 @@
         <v>19</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -3373,13 +3370,13 @@
         <v>19</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -3387,13 +3384,13 @@
         <v>19</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -3401,13 +3398,13 @@
         <v>19</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -3415,13 +3412,13 @@
         <v>19</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -3429,13 +3426,13 @@
         <v>19</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -3443,16 +3440,16 @@
         <v>19</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H61" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I61" s="5" t="s">
         <v>25</v>
@@ -3463,13 +3460,13 @@
         <v>19</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -3477,16 +3474,16 @@
         <v>19</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D63" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F63" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F63" s="3" t="s">
-        <v>90</v>
-      </c>
       <c r="G63" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -3494,16 +3491,16 @@
         <v>19</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -3511,16 +3508,16 @@
         <v>19</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -3528,16 +3525,16 @@
         <v>19</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -3545,16 +3542,16 @@
         <v>19</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -3562,19 +3559,19 @@
         <v>19</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H68" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I68" s="5" t="s">
         <v>25</v>
@@ -3585,19 +3582,19 @@
         <v>19</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H69" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I69" s="5" t="s">
         <v>25</v>
@@ -3608,13 +3605,13 @@
         <v>19</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -3622,16 +3619,16 @@
         <v>19</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H71" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I71" s="5" t="s">
         <v>25</v>
@@ -3642,10 +3639,10 @@
         <v>19</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -3653,16 +3650,16 @@
         <v>19</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D73" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E73" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E73" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="H73" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I73" s="9" t="s">
         <v>25</v>
@@ -3673,10 +3670,10 @@
         <v>19</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -3684,13 +3681,13 @@
         <v>19</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -3698,13 +3695,13 @@
         <v>19</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -3712,13 +3709,13 @@
         <v>19</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -3726,13 +3723,13 @@
         <v>19</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -3740,16 +3737,16 @@
         <v>19</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H79" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I79" s="5" t="s">
         <v>25</v>
@@ -3760,13 +3757,13 @@
         <v>19</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -3774,16 +3771,16 @@
         <v>19</v>
       </c>
       <c r="B81" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H81" t="s">
         <v>45</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E81" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H81" t="s">
-        <v>46</v>
       </c>
       <c r="I81" s="5" t="s">
         <v>25</v>
@@ -3794,13 +3791,13 @@
         <v>19</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
@@ -3808,16 +3805,16 @@
         <v>19</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D83" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E83" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E83" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="H83" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I83" s="9" t="s">
         <v>25</v>
@@ -3828,16 +3825,16 @@
         <v>19</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D84" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E84" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E84" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="H84" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I84" s="5" t="s">
         <v>25</v>
@@ -3848,16 +3845,16 @@
         <v>19</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D85" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E85" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E85" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="H85" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I85" s="5" t="s">
         <v>25</v>
@@ -3868,10 +3865,10 @@
         <v>19</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
@@ -3879,13 +3876,13 @@
         <v>19</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H87" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I87" s="5" t="s">
         <v>25</v>
@@ -3896,13 +3893,13 @@
         <v>19</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H88" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I88" s="5" t="s">
         <v>25</v>
@@ -3913,10 +3910,10 @@
         <v>19</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I89" s="5" t="s">
         <v>27</v>
@@ -3927,10 +3924,10 @@
         <v>19</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I90" s="5" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
CN0804: Ajuste de Esqueleto y carga documento producción digital
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion04/EsqueletoGuion_CN_08_04_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion04/EsqueletoGuion_CN_08_04_CO.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Documents\Aula Planeta Colombia\Repositorios\CienciasNaturales\fuentes\contenidos\grado08\guion04\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="1455" windowWidth="19440" windowHeight="11700" tabRatio="729" activeTab="4"/>
+    <workbookView xWindow="3408" yWindow="1455" windowWidth="19444" windowHeight="11701" tabRatio="729"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -13,13 +18,13 @@
     <sheet name="CUADERNO DEL PROFESOR" sheetId="15" r:id="rId4"/>
     <sheet name="CUADERNO DE ESTUDIO" sheetId="16" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="152511"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -94,9 +99,6 @@
     <t xml:space="preserve">Los seres vivos permanecen en la Tierra gracias a su capacidad de reproducirse. Reconoce las diferentes formas que utilizan los organismos para crean otros semejantes a ellos. </t>
   </si>
   <si>
-    <t>Educación básica secundaria</t>
-  </si>
-  <si>
     <t>Ciencias Naturales</t>
   </si>
   <si>
@@ -329,6 +331,9 @@
   </si>
   <si>
     <t>Refuerza tu aprendizaje: La reproducción de las plantas</t>
+  </si>
+  <si>
+    <t>Educación Básica Secundaria</t>
   </si>
 </sst>
 </file>
@@ -1548,7 +1553,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1558,17 +1563,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="104.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.3984375" customWidth="1"/>
+    <col min="2" max="2" width="104.265625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="15" t="s">
         <v>8</v>
       </c>
@@ -1576,7 +1581,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="15" t="s">
         <v>9</v>
       </c>
@@ -1584,7 +1589,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="15" t="s">
         <v>10</v>
       </c>
@@ -1592,15 +1597,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="15" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="15" t="s">
         <v>1</v>
       </c>
@@ -1608,12 +1613,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="15" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1635,19 +1640,19 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.73046875" customWidth="1"/>
+    <col min="5" max="5" width="20.3984375" customWidth="1"/>
+    <col min="7" max="7" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.73046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
@@ -1667,21 +1672,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
         <v>30</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>31</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>32</v>
       </c>
-      <c r="D2" t="s">
-        <v>33</v>
-      </c>
       <c r="E2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F2">
         <v>4</v>
@@ -1693,245 +1698,245 @@
       <c r="K2"/>
       <c r="L2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
         <v>30</v>
       </c>
-      <c r="B3" t="s">
-        <v>31</v>
-      </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" t="s">
         <v>51</v>
-      </c>
-      <c r="E3" t="s">
-        <v>52</v>
       </c>
       <c r="F3">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F4">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
         <v>39</v>
       </c>
-      <c r="B5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" t="s">
-        <v>40</v>
-      </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F5">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F6">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F7">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" t="s">
         <v>43</v>
       </c>
-      <c r="D8" t="s">
-        <v>44</v>
-      </c>
       <c r="E8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F8">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
         <v>30</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" t="s">
-        <v>32</v>
-      </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F9">
         <v>15</v>
       </c>
       <c r="G9" s="10"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F10">
         <v>16</v>
       </c>
       <c r="G10" s="10"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F11">
         <v>17</v>
       </c>
       <c r="G11" s="10"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F12">
         <v>18</v>
       </c>
       <c r="G12" s="10"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
         <v>30</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>31</v>
       </c>
-      <c r="C13" t="s">
-        <v>32</v>
-      </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F13">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
         <v>30</v>
       </c>
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F14">
         <v>20</v>
@@ -1953,16 +1958,16 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="66.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="66.1328125" customWidth="1"/>
+    <col min="2" max="2" width="14.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="14" t="s">
         <v>3</v>
       </c>
@@ -1973,100 +1978,100 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
         <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>25</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
         <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10">
         <v>22</v>
@@ -2088,7 +2093,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:C27"/>
@@ -2097,14 +2102,14 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="92.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.265625" customWidth="1"/>
+    <col min="3" max="3" width="19.265625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="23.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="11" t="s">
         <v>5</v>
       </c>
@@ -2115,249 +2120,249 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C27" s="6"/>
     </row>
   </sheetData>
@@ -2379,25 +2384,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="615" activePane="bottomLeft"/>
-      <selection pane="bottomLeft"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="618" topLeftCell="A55" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="I74" sqref="I74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="61.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="30.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="64.140625" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.1328125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28.265625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="61.265625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.86328125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="30.86328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.86328125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="64.1328125" customWidth="1"/>
+    <col min="9" max="9" width="17.3984375" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
@@ -2426,15 +2431,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -2442,131 +2447,131 @@
       <c r="G2" s="9"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" s="16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>63</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>64</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>65</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>66</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
@@ -2574,1363 +2579,1363 @@
       <c r="G9" s="9"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E16" s="9"/>
       <c r="F16" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E19" s="9"/>
       <c r="F19" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E23" s="9"/>
       <c r="F23" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>19</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E24" s="9"/>
       <c r="F24" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H24" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="I24" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>29</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>19</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D27" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="G29" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H39" t="s">
+        <v>32</v>
+      </c>
+      <c r="I39" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H40" t="s">
+        <v>79</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H47" t="s">
+        <v>83</v>
+      </c>
+      <c r="I47" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
+        <v>19</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
+        <v>19</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
+        <v>19</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D28" s="9" t="s">
+      <c r="H50" t="s">
+        <v>50</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
+        <v>19</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H52" t="s">
+        <v>98</v>
+      </c>
+      <c r="I52" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
+        <v>19</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
+        <v>19</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
+        <v>19</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
+        <v>19</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>19</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
+        <v>19</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
+        <v>19</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
+        <v>19</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H61" t="s">
+        <v>36</v>
+      </c>
+      <c r="I61" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A62" t="s">
+        <v>19</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A63" t="s">
+        <v>19</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A64" t="s">
+        <v>19</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F64" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="G64" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A65" t="s">
+        <v>19</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A66" t="s">
+        <v>19</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A67" t="s">
+        <v>19</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A68" t="s">
+        <v>19</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H68" t="s">
+        <v>39</v>
+      </c>
+      <c r="I68" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A69" t="s">
+        <v>19</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H69" t="s">
+        <v>53</v>
+      </c>
+      <c r="I69" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A70" t="s">
+        <v>19</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A71" t="s">
+        <v>19</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H71" t="s">
+        <v>54</v>
+      </c>
+      <c r="I71" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A72" t="s">
+        <v>19</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D72" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G29" s="3" t="s">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A73" t="s">
+        <v>19</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H73" t="s">
+        <v>99</v>
+      </c>
+      <c r="I73" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A74" t="s">
+        <v>19</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A75" t="s">
+        <v>19</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A76" t="s">
+        <v>19</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A77" t="s">
+        <v>19</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A78" t="s">
+        <v>19</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A79" t="s">
+        <v>19</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E79" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>19</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G30" s="3" t="s">
+      <c r="H79" t="s">
+        <v>43</v>
+      </c>
+      <c r="I79" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A80" t="s">
+        <v>19</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A81" t="s">
+        <v>19</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H81" t="s">
+        <v>44</v>
+      </c>
+      <c r="I81" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A82" t="s">
+        <v>19</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D82" s="3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>19</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>19</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>19</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G33" s="3" t="s">
+      <c r="E82" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A83" t="s">
+        <v>19</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D83" s="3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>19</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>19</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>19</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>19</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>19</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D38" s="9" t="s">
+      <c r="E83" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E38" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>19</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D39" s="3" t="s">
+      <c r="H83" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I83" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A84" t="s">
+        <v>19</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E84" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E39" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H39" t="s">
-        <v>33</v>
-      </c>
-      <c r="I39" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>19</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D40" s="3" t="s">
+      <c r="H84" t="s">
+        <v>56</v>
+      </c>
+      <c r="I84" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A85" t="s">
+        <v>19</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E85" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E40" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H40" t="s">
-        <v>80</v>
-      </c>
-      <c r="I40" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>19</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>19</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>19</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>19</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>19</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>19</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D46" s="3" t="s">
+      <c r="H85" t="s">
+        <v>57</v>
+      </c>
+      <c r="I85" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A86" t="s">
+        <v>19</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A87" t="s">
+        <v>19</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C87" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E46" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>19</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D47" s="3" t="s">
+      <c r="H87" t="s">
+        <v>46</v>
+      </c>
+      <c r="I87" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A88" t="s">
+        <v>19</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C88" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E47" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H47" t="s">
-        <v>84</v>
-      </c>
-      <c r="I47" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>19</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>19</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>19</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H50" t="s">
-        <v>51</v>
-      </c>
-      <c r="I50" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>19</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>19</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H52" t="s">
-        <v>99</v>
-      </c>
-      <c r="I52" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>19</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>19</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>19</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>19</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>19</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>19</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>19</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>19</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>19</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H61" t="s">
-        <v>37</v>
-      </c>
-      <c r="I61" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>19</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>19</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F63" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="G63" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>19</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F64" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G64" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>19</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F65" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="G65" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>19</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F66" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="G66" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>19</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F67" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="G67" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>19</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F68" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="G68" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H68" t="s">
-        <v>40</v>
-      </c>
-      <c r="I68" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>19</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F69" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="G69" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H69" t="s">
-        <v>54</v>
-      </c>
-      <c r="I69" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>19</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>19</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H71" t="s">
-        <v>55</v>
-      </c>
-      <c r="I71" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>19</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>19</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H73" t="s">
-        <v>100</v>
-      </c>
-      <c r="I73" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>19</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>19</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E75" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>19</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E76" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>19</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E77" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>19</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>19</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E79" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H79" t="s">
-        <v>44</v>
-      </c>
-      <c r="I79" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>19</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>19</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E81" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H81" t="s">
-        <v>45</v>
-      </c>
-      <c r="I81" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>19</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>19</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E83" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H83" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="I83" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>19</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H84" t="s">
-        <v>57</v>
-      </c>
-      <c r="I84" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>19</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E85" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H85" t="s">
+      <c r="H88" t="s">
         <v>58</v>
       </c>
-      <c r="I85" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>19</v>
-      </c>
-      <c r="B86" s="2" t="s">
+      <c r="I88" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A89" t="s">
+        <v>19</v>
+      </c>
+      <c r="B89" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C86" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>19</v>
-      </c>
-      <c r="B87" s="2" t="s">
+      <c r="C89" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I89" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A90" t="s">
+        <v>19</v>
+      </c>
+      <c r="B90" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C87" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H87" t="s">
-        <v>47</v>
-      </c>
-      <c r="I87" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>19</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H88" t="s">
-        <v>59</v>
-      </c>
-      <c r="I88" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>19</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C89" s="2" t="s">
+      <c r="C90" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I89" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>19</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="I90" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Arreglos en la numeración de los recursos
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion04/EsqueletoGuion_CN_08_04_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion04/EsqueletoGuion_CN_08_04_CO.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Documents\Aula Planeta Colombia\Repositorios\CienciasNaturales\fuentes\contenidos\grado08\guion04\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3408" yWindow="1455" windowWidth="19444" windowHeight="11701" tabRatio="729"/>
+    <workbookView xWindow="3405" yWindow="1455" windowWidth="19440" windowHeight="11700" tabRatio="729" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -18,13 +13,13 @@
     <sheet name="CUADERNO DEL PROFESOR" sheetId="15" r:id="rId4"/>
     <sheet name="CUADERNO DE ESTUDIO" sheetId="16" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -99,6 +94,9 @@
     <t xml:space="preserve">Los seres vivos permanecen en la Tierra gracias a su capacidad de reproducirse. Reconoce las diferentes formas que utilizan los organismos para crean otros semejantes a ellos. </t>
   </si>
   <si>
+    <t>Educación básica secundaria</t>
+  </si>
+  <si>
     <t>Ciencias Naturales</t>
   </si>
   <si>
@@ -331,9 +329,6 @@
   </si>
   <si>
     <t>Refuerza tu aprendizaje: La reproducción de las plantas</t>
-  </si>
-  <si>
-    <t>Educación Básica Secundaria</t>
   </si>
 </sst>
 </file>
@@ -1553,7 +1548,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1563,17 +1558,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.3984375" customWidth="1"/>
-    <col min="2" max="2" width="104.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="104.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>8</v>
       </c>
@@ -1581,7 +1576,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>9</v>
       </c>
@@ -1589,7 +1584,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>10</v>
       </c>
@@ -1597,15 +1592,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>1</v>
       </c>
@@ -1613,12 +1608,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1640,19 +1635,19 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.73046875" customWidth="1"/>
-    <col min="5" max="5" width="20.3984375" customWidth="1"/>
-    <col min="7" max="7" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.1328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.73046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
@@ -1672,21 +1667,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F2">
         <v>4</v>
@@ -1698,245 +1693,245 @@
       <c r="K2"/>
       <c r="L2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F3">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
         <v>38</v>
       </c>
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>37</v>
       </c>
-      <c r="D4" t="s">
-        <v>36</v>
-      </c>
       <c r="E4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F4">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
         <v>38</v>
       </c>
-      <c r="B5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" t="s">
-        <v>37</v>
-      </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F5">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
         <v>38</v>
       </c>
-      <c r="B6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" t="s">
-        <v>37</v>
-      </c>
       <c r="D6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" t="s">
         <v>53</v>
-      </c>
-      <c r="E6" t="s">
-        <v>52</v>
       </c>
       <c r="F6">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
         <v>38</v>
       </c>
-      <c r="B7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" t="s">
-        <v>37</v>
-      </c>
       <c r="D7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F7">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F8">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F9">
         <v>15</v>
       </c>
       <c r="G9" s="10"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F10">
         <v>16</v>
       </c>
       <c r="G10" s="10"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" t="s">
         <v>56</v>
-      </c>
-      <c r="E11" t="s">
-        <v>55</v>
       </c>
       <c r="F11">
         <v>17</v>
       </c>
       <c r="G11" s="10"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F12">
         <v>18</v>
       </c>
       <c r="G12" s="10"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>30</v>
       </c>
-      <c r="C13" t="s">
+      <c r="B14" t="s">
         <v>31</v>
       </c>
-      <c r="D13" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" t="s">
-        <v>49</v>
-      </c>
-      <c r="F13">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" t="s">
-        <v>30</v>
-      </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F14">
         <v>20</v>
@@ -1958,16 +1953,16 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.1328125" customWidth="1"/>
-    <col min="2" max="2" width="14.73046875" customWidth="1"/>
+    <col min="1" max="1" width="66.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>3</v>
       </c>
@@ -1978,100 +1973,100 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
         <v>27</v>
-      </c>
-      <c r="B4" t="s">
-        <v>26</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C6">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C8">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C9">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C10">
         <v>22</v>
@@ -2093,7 +2088,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:C27"/>
@@ -2102,14 +2097,14 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="92.265625" customWidth="1"/>
-    <col min="3" max="3" width="19.265625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>5</v>
       </c>
@@ -2120,249 +2115,249 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C27" s="6"/>
     </row>
   </sheetData>
@@ -2384,25 +2379,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="618" topLeftCell="A55" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="I74" sqref="I74"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="615" activePane="bottomLeft"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.1328125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="28.265625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="61.265625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.86328125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="30.86328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.86328125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="64.1328125" customWidth="1"/>
-    <col min="9" max="9" width="17.3984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="61.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="30.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="64.140625" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
@@ -2431,15 +2426,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -2447,131 +2442,131 @@
       <c r="G2" s="9"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" s="16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
@@ -2579,1363 +2574,1363 @@
       <c r="G9" s="9"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E16" s="9"/>
       <c r="F16" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E19" s="9"/>
       <c r="F19" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E23" s="9"/>
       <c r="F23" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>19</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E24" s="9"/>
       <c r="F24" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H24" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I24" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="I24" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>19</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D27" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F36" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D28" s="9" t="s">
+      <c r="G36" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F37" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
-        <v>19</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
-        <v>19</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
-        <v>19</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="F32" s="3" t="s">
+      <c r="G37" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H39" t="s">
+        <v>33</v>
+      </c>
+      <c r="I39" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H40" t="s">
+        <v>80</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H47" t="s">
+        <v>84</v>
+      </c>
+      <c r="I47" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>19</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>19</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>19</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H50" t="s">
+        <v>51</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>19</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H52" t="s">
+        <v>99</v>
+      </c>
+      <c r="I52" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>19</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>19</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>19</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>19</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>19</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>19</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>19</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>19</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H61" t="s">
+        <v>37</v>
+      </c>
+      <c r="I61" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>19</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>19</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>19</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F64" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="G32" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
-        <v>19</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
-        <v>19</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
-        <v>19</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
-      <c r="A36" t="s">
-        <v>19</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
-        <v>19</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G37" s="3" t="s">
+      <c r="G64" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>19</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>19</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>19</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>19</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H68" t="s">
+        <v>40</v>
+      </c>
+      <c r="I68" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>19</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H69" t="s">
+        <v>54</v>
+      </c>
+      <c r="I69" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>19</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>19</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E71" s="3" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
-        <v>19</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
-        <v>19</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E39" s="3" t="s">
+      <c r="H71" t="s">
+        <v>55</v>
+      </c>
+      <c r="I71" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>19</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D72" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H39" t="s">
-        <v>32</v>
-      </c>
-      <c r="I39" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
-        <v>19</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E40" s="3" t="s">
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>19</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D73" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H40" t="s">
-        <v>79</v>
-      </c>
-      <c r="I40" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
-        <v>19</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
-        <v>19</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
-        <v>19</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
-        <v>19</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D44" s="3" t="s">
+      <c r="E73" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H73" t="s">
+        <v>100</v>
+      </c>
+      <c r="I73" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>19</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>19</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>19</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>19</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E77" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E44" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A45" t="s">
-        <v>19</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A46" t="s">
-        <v>19</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A47" t="s">
-        <v>19</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E47" s="3" t="s">
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>19</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>19</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H79" t="s">
+        <v>44</v>
+      </c>
+      <c r="I79" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>19</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>19</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H81" t="s">
+        <v>45</v>
+      </c>
+      <c r="I81" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>19</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D82" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H47" t="s">
-        <v>83</v>
-      </c>
-      <c r="I47" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A48" t="s">
-        <v>19</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A49" t="s">
-        <v>19</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A50" t="s">
-        <v>19</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H50" t="s">
-        <v>50</v>
-      </c>
-      <c r="I50" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A51" t="s">
-        <v>19</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A52" t="s">
-        <v>19</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E52" s="2" t="s">
+      <c r="E82" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>19</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D83" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H52" t="s">
+      <c r="E83" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H83" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I83" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>19</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H84" t="s">
+        <v>57</v>
+      </c>
+      <c r="I84" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>19</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H85" t="s">
+        <v>58</v>
+      </c>
+      <c r="I85" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>19</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>19</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H87" t="s">
+        <v>47</v>
+      </c>
+      <c r="I87" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>19</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H88" t="s">
+        <v>59</v>
+      </c>
+      <c r="I88" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>19</v>
+      </c>
+      <c r="B89" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="I52" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A53" t="s">
-        <v>19</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
-      <c r="A54" t="s">
-        <v>19</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A55" t="s">
-        <v>19</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A56" t="s">
-        <v>19</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A57" t="s">
-        <v>19</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A58" t="s">
-        <v>19</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A59" t="s">
-        <v>19</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A60" t="s">
-        <v>19</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A61" t="s">
-        <v>19</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H61" t="s">
-        <v>36</v>
-      </c>
-      <c r="I61" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A62" t="s">
-        <v>19</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A63" t="s">
-        <v>19</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F63" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="G63" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A64" t="s">
-        <v>19</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F64" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G64" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A65" t="s">
-        <v>19</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F65" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="G65" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A66" t="s">
-        <v>19</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F66" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="G66" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A67" t="s">
-        <v>19</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F67" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="G67" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A68" t="s">
-        <v>19</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F68" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="G68" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H68" t="s">
-        <v>39</v>
-      </c>
-      <c r="I68" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A69" t="s">
-        <v>19</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F69" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="G69" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H69" t="s">
-        <v>53</v>
-      </c>
-      <c r="I69" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A70" t="s">
-        <v>19</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A71" t="s">
-        <v>19</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H71" t="s">
-        <v>54</v>
-      </c>
-      <c r="I71" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A72" t="s">
-        <v>19</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A73" t="s">
-        <v>19</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H73" t="s">
-        <v>99</v>
-      </c>
-      <c r="I73" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A74" t="s">
-        <v>19</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A75" t="s">
-        <v>19</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E75" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A76" t="s">
-        <v>19</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E76" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A77" t="s">
-        <v>19</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E77" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A78" t="s">
-        <v>19</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A79" t="s">
-        <v>19</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E79" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H79" t="s">
-        <v>43</v>
-      </c>
-      <c r="I79" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A80" t="s">
-        <v>19</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A81" t="s">
-        <v>19</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E81" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H81" t="s">
-        <v>44</v>
-      </c>
-      <c r="I81" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A82" t="s">
-        <v>19</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A83" t="s">
-        <v>19</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E83" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H83" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I83" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A84" t="s">
-        <v>19</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H84" t="s">
-        <v>56</v>
-      </c>
-      <c r="I84" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A85" t="s">
-        <v>19</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E85" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H85" t="s">
-        <v>57</v>
-      </c>
-      <c r="I85" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A86" t="s">
-        <v>19</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A87" t="s">
-        <v>19</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H87" t="s">
-        <v>46</v>
-      </c>
-      <c r="I87" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A88" t="s">
-        <v>19</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H88" t="s">
-        <v>58</v>
-      </c>
-      <c r="I88" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A89" t="s">
-        <v>19</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>97</v>
-      </c>
       <c r="C89" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I89" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>19</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I90" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>